<commit_message>
edits for new england report post 12
</commit_message>
<xml_diff>
--- a/new_england_natgas.xlsx
+++ b/new_england_natgas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredkramer/Documents/python/hummingbird/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADA1986-1582-824F-BCED-CA61B0EB408C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CA46A3-2B02-EB45-B5B6-82DDED8F36B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" xr2:uid="{81DA864C-AB67-0143-8895-4CE114A53937}"/>
   </bookViews>
@@ -16663,6 +16663,7 @@
         <c:axId val="1601412736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="3.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -17360,12 +17361,12 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -17714,8 +17715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4636457-02C7-E649-93F5-C7A32DDA484B}">
   <dimension ref="A1:I879"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E9" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>